<commit_message>
--- TOKEN ONLINE ---
-- BUG --
platformio  > v4.4.0 > bug dma, bluetooth callback, wifi disconnect
solved: - change to espcore arduino 2.0.3-2.0.4
        - platformio v4.4.0
        - editing wifigeneric.c STA_NOTCONNECT

-- LOW TOKEN SOUND--
- fixing detection low token frequency
- penambahan variabel frequency peak
- kirim notification api dengan image

-- WIFI
- fixing disconnect dari wifi(fix dengan edit wifigeneric STA_NOTCONNECT)
- tambah proccess reconnect

-- SETTING
- penambahan setingan tipe, dengan value waktu untuk capture status,
  nominal, frekuensi peak sesuai tipe, alarm (bluetooth)

-- PROCCESS
- ganti logika isi token dengan millis(). prev dengan delay.
- tambah validasi suara
- ganti interval alarm dari mqtt

--- TOKEN ONLINE ---
</commit_message>
<xml_diff>
--- a/esp32_inmp441/perhitungan.xlsx
+++ b/esp32_inmp441/perhitungan.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PlatformIO\Projects\esp32_inmp441\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742F0C1F-1A9F-42F5-AEBE-353835831DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A2BA7B-3AFD-4D06-8CF8-21478D42AEC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="315" windowWidth="15375" windowHeight="9480" xr2:uid="{D108D1C8-44D8-4858-9651-5F526541ED36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{D108D1C8-44D8-4858-9651-5F526541ED36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t xml:space="preserve">Freq Sampling </t>
   </si>
@@ -119,13 +120,76 @@
   </si>
   <si>
     <t>itron kantor</t>
+  </si>
+  <si>
+    <t>melcoinda gagal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bin1 </t>
+  </si>
+  <si>
+    <t>itron kantor gagal</t>
+  </si>
+  <si>
+    <t>COUNTER BENAR</t>
+  </si>
+  <si>
+    <t>counter gagal</t>
+  </si>
+  <si>
+    <t>TIME ALARM</t>
+  </si>
+  <si>
+    <t>MEREK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itron pak ferdi </t>
+  </si>
+  <si>
+    <t>itron ace9000 kantor(terbuka)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">melcoinda </t>
+  </si>
+  <si>
+    <t>hexing hxe116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanxing </t>
+  </si>
+  <si>
+    <t>smartmeter</t>
+  </si>
+  <si>
+    <t>ACTUAL</t>
+  </si>
+  <si>
+    <t>SENSOR</t>
+  </si>
+  <si>
+    <t>TIME BENAR</t>
+  </si>
+  <si>
+    <t>TIME GAGAL</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>3 beep</t>
+  </si>
+  <si>
+    <t>1 beep</t>
+  </si>
+  <si>
+    <t>1 beep long</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,13 +203,37 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,9 +248,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2390,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6DE7C1-7E52-4DE1-B00C-23F964BE36BE}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,11 +2493,12 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2420,7 +2512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2431,7 +2523,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2450,7 +2542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2471,7 +2563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2490,13 +2582,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G6">
         <f>21.33*48</f>
         <v>1023.8399999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2515,8 +2607,14 @@
       <c r="I7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2535,8 +2633,20 @@
       <c r="I8">
         <v>3737</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>3830</v>
+      </c>
+      <c r="M8">
+        <v>3830</v>
+      </c>
+      <c r="P8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2555,8 +2665,20 @@
       <c r="I9">
         <v>4264</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>4170</v>
+      </c>
+      <c r="M9">
+        <v>4350</v>
+      </c>
+      <c r="P9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9">
+        <v>5165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2577,11 +2699,30 @@
         <v>168.62261899500598</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10" si="1">I8/$C$4</f>
+        <f t="shared" ref="I10:K10" si="1">I8/$C$4</f>
         <v>169.1204313430857</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>173.32920846775977</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="2">M8/$C$4</f>
+        <v>173.32920846775977</v>
+      </c>
+      <c r="P10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10" si="3">Q8/$C$4</f>
+        <v>115.13041941043886</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2602,16 +2743,35 @@
         <v>193.96579307906484</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11" si="2">I9/$C$4</f>
+        <f t="shared" ref="I11:K11" si="4">I9/$C$4</f>
         <v>192.97016838290537</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>188.71613559022407</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11" si="5">M9/$C$4</f>
+        <v>196.8621558315287</v>
+      </c>
+      <c r="P11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ref="Q11" si="6">Q9/$C$4</f>
+        <v>233.74552525743582</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>23</v>
       </c>
@@ -2622,7 +2782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>109</v>
       </c>
@@ -2639,13 +2799,16 @@
         <v>240</v>
       </c>
       <c r="K15">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="L15">
         <v>230</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C16">
         <f>C15/$D$3</f>
         <v>2.4085380859375003</v>
@@ -2668,25 +2831,354 @@
       </c>
       <c r="K16">
         <f>K15/$D$3</f>
-        <v>5.082236328125</v>
+        <v>5.7893300781250003</v>
       </c>
       <c r="L16">
         <f>L15/$D$3</f>
         <v>5.082236328125</v>
       </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f>M15/$D$3</f>
+        <v>2.3201513671875</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>270</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E18">
         <f>E17/$D$3</f>
         <v>5.966103515625</v>
       </c>
     </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20">
+        <f>320-18</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="I21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22">
+        <v>302</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:K26" si="7">I22/$D$3</f>
+        <v>6.6731972656250003</v>
+      </c>
+      <c r="L22">
+        <f>ROUND(K22,1)</f>
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23">
+        <v>261</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
+        <v>5.7672333984374999</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:L27" si="8">ROUND(K23,1)</f>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24">
+        <v>88</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="7"/>
+        <v>1.9445078125000002</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="8"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25">
+        <v>560</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="7"/>
+        <v>12.374140625000001</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="8"/>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26">
+        <v>112</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="7"/>
+        <v>2.4748281250000002</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27">
+        <v>556</v>
+      </c>
+      <c r="K27">
+        <f>I27/$D$3</f>
+        <v>12.285753906250001</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="8"/>
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="I31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32">
+        <v>227</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ref="K32:K36" si="9">I32/$D$3</f>
+        <v>5.0159462890625006</v>
+      </c>
+      <c r="L32">
+        <f>ROUND(K32,1)</f>
+        <v>5</v>
+      </c>
+      <c r="M32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33">
+        <v>227</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="9"/>
+        <v>5.0159462890625006</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ref="L33:L37" si="10">ROUND(K33,1)</f>
+        <v>5</v>
+      </c>
+      <c r="M33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34">
+        <v>73</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="9"/>
+        <v>1.6130576171875</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="10"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35">
+        <v>800</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="9"/>
+        <v>17.677343750000002</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="10"/>
+        <v>17.7</v>
+      </c>
+      <c r="M35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M40">
+        <f>320-18</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42">
+        <v>227</v>
+      </c>
+      <c r="K42">
+        <f t="shared" ref="K42:K46" si="11">I42/$D$3</f>
+        <v>5.0159462890625006</v>
+      </c>
+      <c r="L42">
+        <f>ROUND(K42,1)</f>
+        <v>5</v>
+      </c>
+      <c r="M42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43">
+        <v>227</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="11"/>
+        <v>5.0159462890625006</v>
+      </c>
+      <c r="L43">
+        <f t="shared" ref="L43:L47" si="12">ROUND(K43,1)</f>
+        <v>5</v>
+      </c>
+      <c r="M43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44">
+        <v>70</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="11"/>
+        <v>1.5467675781250001</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="12"/>
+        <v>1.5</v>
+      </c>
+      <c r="M44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45">
+        <v>1024</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="11"/>
+        <v>22.627000000000002</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="12"/>
+        <v>22.6</v>
+      </c>
+      <c r="M45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3037,4 +3529,145 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A755C15-CC66-45B5-B59D-2D5704245F28}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>99-B3</f>
+        <v>59</v>
+      </c>
+      <c r="D4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>158-99</f>
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <f>118-D4</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <f>193-118</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>118-B6</f>
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <f>281-193</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>158-118</f>
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <f>355-281</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>199-158</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>258-199</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>308-258</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>AVERAGE(B2:B11)</f>
+        <v>50.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
jumat 17 feb 2023 pagi - ganti metode capture   - metode = capture ke file system->simpan ke filesystem->selesai - ganti metode upload   - metode = tidak upload ketika proses capture   - ketika sudah tercapture semua, flag upload hidup   - ketika flag upload hidup, check wifi untuk cek koneksi kemudian upload     semua file bukti token(nominal,saldo,status).   - flag upload akan false ketika upload mendapatkan pesan sukses(HTTP 200 OK) - ganti metode alarm   - selalu cek frequensi walaupun belum timout untuk alarm   - ketika waktunya kirim alarm dan counter deteksi kurang maka timout alarm akan reset   - soundlooping terus cek frekuensi, ketika timoutalarm enable maka langsung cek berapa     nilai counter dan kemudia kirim alarm serta reset semua variable. - ganti metode reconnect wifi DONE:   - capture file system   - upload file system   - disconnect new metode   - alarm new metode NOT FIX:   - LOG file system
</commit_message>
<xml_diff>
--- a/esp32_inmp441/perhitungan.xlsx
+++ b/esp32_inmp441/perhitungan.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PlatformIO\Projects\esp32_inmp441\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A2BA7B-3AFD-4D06-8CF8-21478D42AEC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A2F176-209E-495C-88D9-B781B3D3D18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{D108D1C8-44D8-4858-9651-5F526541ED36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{D108D1C8-44D8-4858-9651-5F526541ED36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t xml:space="preserve">Freq Sampling </t>
   </si>
@@ -183,6 +184,12 @@
   </si>
   <si>
     <t>1 beep long</t>
+  </si>
+  <si>
+    <t>BENAR (lower)</t>
+  </si>
+  <si>
+    <t>GAGAL (upper)</t>
   </si>
 </sst>
 </file>
@@ -2483,8 +2490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6DE7C1-7E52-4DE1-B00C-23F964BE36BE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,7 +3003,7 @@
         <v>227</v>
       </c>
       <c r="K32">
-        <f t="shared" ref="K32:K36" si="9">I32/$D$3</f>
+        <f t="shared" ref="K32:K35" si="9">I32/$D$3</f>
         <v>5.0159462890625006</v>
       </c>
       <c r="L32">
@@ -3019,7 +3026,7 @@
         <v>5.0159462890625006</v>
       </c>
       <c r="L33">
-        <f t="shared" ref="L33:L37" si="10">ROUND(K33,1)</f>
+        <f t="shared" ref="L33:L35" si="10">ROUND(K33,1)</f>
         <v>5</v>
       </c>
       <c r="M33" t="s">
@@ -3099,7 +3106,7 @@
         <v>227</v>
       </c>
       <c r="K42">
-        <f t="shared" ref="K42:K46" si="11">I42/$D$3</f>
+        <f t="shared" ref="K42:K45" si="11">I42/$D$3</f>
         <v>5.0159462890625006</v>
       </c>
       <c r="L42">
@@ -3122,7 +3129,7 @@
         <v>5.0159462890625006</v>
       </c>
       <c r="L43">
-        <f t="shared" ref="L43:L47" si="12">ROUND(K43,1)</f>
+        <f t="shared" ref="L43:L45" si="12">ROUND(K43,1)</f>
         <v>5</v>
       </c>
       <c r="M43" t="s">
@@ -3184,6 +3191,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE815256-F0C6-4D59-B2F0-AD9B193E038C}">
+  <dimension ref="B1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD00866-AE56-4667-9857-E4DBC38A7D2C}">
   <dimension ref="A1:M54"/>
   <sheetViews>
@@ -3531,7 +3612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A755C15-CC66-45B5-B59D-2D5704245F28}">
   <dimension ref="A1:D12"/>
   <sheetViews>

</xml_diff>